<commit_message>
eps, cndh, and payload component implementation
</commit_message>
<xml_diff>
--- a/documentation/Component Attributes.xlsx
+++ b/documentation/Component Attributes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a.aguilar/Documents/GitHub/DMASpy/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BE2A3B3-80C1-B44B-BDB0-7AA4A68E2C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7764A1-EAAF-EC4F-BF7A-E596A6892B4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{4E23E951-76E0-744F-B01E-BC7D7E9F9B86}"/>
   </bookViews>
@@ -35,10 +35,110 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="29">
+  <si>
+    <t>EPS</t>
+  </si>
+  <si>
+    <t>Battery</t>
+  </si>
+  <si>
+    <t>Solar Panel</t>
+  </si>
+  <si>
+    <t>GNC</t>
+  </si>
+  <si>
+    <t>State Attribute</t>
+  </si>
+  <si>
+    <t>IMU</t>
+  </si>
+  <si>
+    <t>Sun Detector</t>
+  </si>
+  <si>
+    <t>GPS</t>
+  </si>
+  <si>
+    <t>Comms</t>
+  </si>
+  <si>
+    <t>Transceiver</t>
+  </si>
+  <si>
+    <t>Payload</t>
+  </si>
+  <si>
+    <t>Instrument i</t>
+  </si>
+  <si>
+    <t>Power Consumed</t>
+  </si>
+  <si>
+    <t>Power Supplied</t>
+  </si>
+  <si>
+    <t>Power Generated</t>
+  </si>
+  <si>
+    <t>Energy Stored</t>
+  </si>
+  <si>
+    <t>Energy Capacity</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Power Generation Degradation</t>
+  </si>
+  <si>
+    <t>Attitude Quaternion Vector</t>
+  </si>
+  <si>
+    <t>Eclipse Status</t>
+  </si>
+  <si>
+    <t>Component Status</t>
+  </si>
+  <si>
+    <t>Position Vector</t>
+  </si>
+  <si>
+    <t>Velocity Vector</t>
+  </si>
+  <si>
+    <t>Buffer Capacity</t>
+  </si>
+  <si>
+    <t>Buffer Allocated</t>
+  </si>
+  <si>
+    <t>Data Rate In</t>
+  </si>
+  <si>
+    <t>Data Rate Out</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -66,8 +166,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,14 +483,452 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71649790-4C62-C443-8AD7-EFC354F8F903}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
separated messages and tasks into two separate files
</commit_message>
<xml_diff>
--- a/documentation/Component Attributes.xlsx
+++ b/documentation/Component Attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a.aguilar/Documents/GitHub/DMASpy/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5693E85C-9329-7749-837B-BEB2CCFD82A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C35AF7-03EA-1A47-B823-8BC30C5813E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25520" yWindow="4980" windowWidth="24840" windowHeight="17440" activeTab="1" xr2:uid="{4E23E951-76E0-744F-B01E-BC7D7E9F9B86}"/>
+    <workbookView xWindow="1740" yWindow="3780" windowWidth="24840" windowHeight="17440" activeTab="3" xr2:uid="{4E23E951-76E0-744F-B01E-BC7D7E9F9B86}"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="118">
   <si>
     <t>EPS</t>
   </si>
@@ -141,12 +141,6 @@
     <t>Task Handler</t>
   </si>
   <si>
-    <t>Message Handler</t>
-  </si>
-  <si>
-    <t>Maintnance Task Hander</t>
-  </si>
-  <si>
     <t>Critical Check</t>
   </si>
   <si>
@@ -394,6 +388,12 @@
   </si>
   <si>
     <t xml:space="preserve">Allocates message in buffer. If buffer is full, it rejects the task. If accepted, the component samples the environment until the target is accessible. Once this is done, it transmits the message. </t>
+  </si>
+  <si>
+    <t>Decompose Subsystem Task</t>
+  </si>
+  <si>
+    <t>Decompose Platform Task</t>
   </si>
 </sst>
 </file>
@@ -1241,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1C36E08-AF04-6844-8281-384705BE1BC6}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1267,13 +1267,13 @@
         <v>29</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>31</v>
@@ -1282,24 +1282,24 @@
         <v>32</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="K1" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
         <v>17</v>
@@ -1334,7 +1334,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -1367,7 +1367,7 @@
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
@@ -1402,7 +1402,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
@@ -1434,7 +1434,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
@@ -1449,7 +1449,7 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F7" t="s">
         <v>17</v>
@@ -1498,7 +1498,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
@@ -1531,7 +1531,7 @@
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
@@ -1599,45 +1599,45 @@
         <v>29</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="F1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>55</v>
-      </c>
       <c r="F2" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>17</v>
@@ -1645,25 +1645,25 @@
     </row>
     <row r="3" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>56</v>
-      </c>
       <c r="F3" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H3" s="8" t="s">
         <v>17</v>
@@ -1671,25 +1671,25 @@
     </row>
     <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>60</v>
-      </c>
       <c r="F4" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>17</v>
@@ -1697,25 +1697,25 @@
     </row>
     <row r="5" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>63</v>
-      </c>
       <c r="F5" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>17</v>
@@ -1725,19 +1725,19 @@
       <c r="A6" s="12"/>
       <c r="B6" s="11"/>
       <c r="C6" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>17</v>
@@ -1748,22 +1748,22 @@
         <v>10</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H7" s="8" t="s">
         <v>17</v>
@@ -1771,25 +1771,25 @@
     </row>
     <row r="8" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>78</v>
-      </c>
       <c r="G8" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H8" s="8" t="s">
         <v>17</v>
@@ -1801,19 +1801,19 @@
         <v>5</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>81</v>
-      </c>
       <c r="G9" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>17</v>
@@ -1824,22 +1824,22 @@
         <v>0</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C10" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="8" t="s">
+      <c r="F10" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>95</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>97</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>17</v>
@@ -1850,22 +1850,22 @@
         <v>8</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C11" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>116</v>
-      </c>
       <c r="F11" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>115</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>117</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>17</v>
@@ -1883,10 +1883,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87581E83-74CA-A741-B44A-95BB95D611E9}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1894,72 +1894,66 @@
     <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>34</v>
+        <v>116</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
     </row>
   </sheetData>
@@ -1992,36 +1986,36 @@
         <v>30</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>50</v>
-      </c>
       <c r="D1" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>99</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -2029,33 +2023,33 @@
         <v>10</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>107</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>111</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="119" x14ac:dyDescent="0.2">
@@ -2063,16 +2057,16 @@
         <v>0</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
engineering module and platform sim in separate files
</commit_message>
<xml_diff>
--- a/documentation/Component Attributes.xlsx
+++ b/documentation/Component Attributes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a.aguilar/Documents/GitHub/DMASpy/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4C836C-5CBE-1B4B-A8E3-F149EBC63212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689F202C-A23E-6D49-BFFF-3E25FDE12574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="3780" windowWidth="24840" windowHeight="17440" activeTab="1" xr2:uid="{4E23E951-76E0-744F-B01E-BC7D7E9F9B86}"/>
+    <workbookView xWindow="1740" yWindow="3780" windowWidth="24840" windowHeight="17440" activeTab="3" xr2:uid="{4E23E951-76E0-744F-B01E-BC7D7E9F9B86}"/>
   </bookViews>
   <sheets>
     <sheet name="Attributes" sheetId="1" r:id="rId1"/>
@@ -1263,7 +1263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1C36E08-AF04-6844-8281-384705BE1BC6}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -1928,7 +1928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87581E83-74CA-A741-B44A-95BB95D611E9}">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>

</xml_diff>